<commit_message>
add Discord; fix error dir in scene.xlsx
Former-commit-id: b8ee07ae6ab2a0978d1eb50996bc106e864b675c [formerly 154ad50fa7544ba42f8ceaa8a61db0d1d1d48e96] [formerly 902d02a30304addeb00dcbf4a263cc64d2ba6b8a [formerly 12ea6197546c50804f7a86898c7b68ce34035022]]
Former-commit-id: 73edb3f127a43c97e81d3e8a752c46c3ba82d0f9 [formerly df2450855d695dccd6b2fb8460e670a439316526]
Former-commit-id: bffe2b54463c4d2c3787391503301228f692ee29
</commit_message>
<xml_diff>
--- a/Bin/Server/resource/excel/Scene.xlsx
+++ b/Bin/Server/resource/excel/Scene.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARK\Bin\Server\resource\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARK\Bin\Server\resource\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -229,7 +229,7 @@
     <t>34.10933,1.165174,11.49214</t>
   </si>
   <si>
-    <t>../resource/Ini/Scene/1.xml</t>
+    <t>../resource/ini/Scene/1.xml</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -243,13 +243,17 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>/Ini/Scene/2.xml</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>../resource</t>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i</t>
     </r>
     <r>
       <rPr>
@@ -258,7 +262,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>/Ini/Scene/3.xml</t>
+      <t>ni/Scene/2.xml</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -273,13 +277,17 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>/Ini/Scene/4.xml</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>../resource</t>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i</t>
     </r>
     <r>
       <rPr>
@@ -288,7 +296,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>/Ini/Scene/5.xml</t>
+      <t>ni/Scene/3.xml</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -303,7 +311,94 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>/Ini/Scene/6.xml</t>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ni/Scene/4.xml</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../resource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ni/Scene/5.xml</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../resource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ni/Scene/6.xml</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -884,7 +979,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
rename resource/struct as resource/schema; fix invalid netclient id; change process name
Former-commit-id: 062b3dedd9f1c559f133533174aee99966acb394 [formerly 1cbf5378fa4c465fa134093a81af08ac5b493b7e] [formerly 9c88feab6b47a9d623bd63ca1702426cf1e68089 [formerly 7a012fe2ca3c194a61c59e8131884f2fc8ea712d]]
Former-commit-id: ff2ead0e50d1089ea90d8dee6f885da39a013de6 [formerly b811e039a9f4cdff44528945f60fa9721ad66a51]
Former-commit-id: c482834a68fe0977f7540457291cac6a39e21078
</commit_message>
<xml_diff>
--- a/Bin/Server/resource/excel/Scene.xlsx
+++ b/Bin/Server/resource/excel/Scene.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARK\Bin\Server\resource\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\ARK\Bin\Server\resource\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8EAC1F64-1C58-4302-89EA-6FBC479BF04E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28692" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode" sheetId="1" r:id="rId1"/>
@@ -19,8 +20,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -229,7 +230,7 @@
     <t>34.10933,1.165174,11.49214</t>
   </si>
   <si>
-    <t>../resource/ini/Scene/1.xml</t>
+    <t>../resource/res/Scene/1.xml</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -253,7 +254,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>i</t>
+      <t>res</t>
     </r>
     <r>
       <rPr>
@@ -262,7 +263,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>ni/Scene/2.xml</t>
+      <t>/Scene/2.xml</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -287,7 +288,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>i</t>
+      <t>res</t>
     </r>
     <r>
       <rPr>
@@ -296,7 +297,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>ni/Scene/3.xml</t>
+      <t>/Scene/4.xml</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -321,7 +322,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>i</t>
+      <t>res</t>
     </r>
     <r>
       <rPr>
@@ -330,7 +331,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>ni/Scene/4.xml</t>
+      <t>/Scene/3.xml</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -355,7 +356,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>i</t>
+      <t>res</t>
     </r>
     <r>
       <rPr>
@@ -364,7 +365,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>ni/Scene/5.xml</t>
+      <t>/Scene/5.xml</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -389,7 +390,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>i</t>
+      <t>res</t>
     </r>
     <r>
       <rPr>
@@ -398,7 +399,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>ni/Scene/6.xml</t>
+      <t>/Scene/6.xml</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -406,7 +407,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -636,6 +637,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -655,7 +724,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -975,30 +1044,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="12.75" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="17.125" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="8.875" customWidth="1"/>
-    <col min="9" max="11" width="27.25" customWidth="1"/>
-    <col min="12" max="12" width="9.375" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="9" max="11" width="27.21875" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="13.25" customWidth="1"/>
+    <col min="14" max="15" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -1098,7 +1167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -1148,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -1198,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -1248,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1298,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
@@ -1348,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>24</v>
       </c>
@@ -1388,7 +1457,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>35</v>
       </c>
@@ -1438,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>42</v>
       </c>
@@ -1488,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>45</v>
       </c>
@@ -1505,7 +1574,7 @@
         <v>200</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>47</v>
@@ -1538,7 +1607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>50</v>
       </c>
@@ -1555,7 +1624,7 @@
         <v>200</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>47</v>
@@ -1588,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>52</v>
       </c>
@@ -1638,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>58</v>
       </c>
@@ -1691,10 +1760,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:I7 J7:P7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:I7 J7:P7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>